<commit_message>
system: modifikasi js landing page map section
</commit_message>
<xml_diff>
--- a/resources/views/backyard/sigarang/report/price_report_template.xlsx
+++ b/resources/views/backyard/sigarang/report/price_report_template.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Bulan</t>
   </si>
   <si>
-    <t xml:space="preserve">[d.month]</t>
+    <t xml:space="preserve">[d.start_date] – [d.end_date]</t>
   </si>
   <si>
     <t xml:space="preserve">Nama Barang</t>
@@ -320,9 +320,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1860840</xdr:colOff>
+      <xdr:colOff>1860480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -336,7 +336,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1047960" y="0"/>
-          <a:ext cx="812880" cy="610200"/>
+          <a:ext cx="812520" cy="609840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -359,7 +359,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
system: modifikasi template laporan harga dan stok
</commit_message>
<xml_diff>
--- a/resources/views/backyard/sigarang/report/price_report_template.xlsx
+++ b/resources/views/backyard/sigarang/report/price_report_template.xlsx
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">Pemerintah Kabupaten Sampang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinas Koperasi, Perindustrian dan Perdagangan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jl Diponogoro No 52 A Telp. (0323) 321066 - 323250 FAX (0323) 323250</t>
+  </si>
   <si>
     <t xml:space="preserve">Laporan Dinamika Harga Barang</t>
   </si>
@@ -63,7 +72,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -99,6 +108,30 @@
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -163,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -173,6 +206,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -264,15 +309,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1047960</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1860840</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>24120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1047960" y="0"/>
+          <a:ext cx="812880" cy="610200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -283,47 +370,65 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -334,5 +439,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>